<commit_message>
added Approval ID in Advanced Search
</commit_message>
<xml_diff>
--- a/substance_dictionary/dictionary_current_all_entities.xlsx
+++ b/substance_dictionary/dictionary_current_all_entities.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GSRSFrontend\substance_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BE70AD-6EFD-4A34-95D4-54808D990E52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67393906-7013-4AA3-8A83-28CB275EBD9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="312" windowWidth="19836" windowHeight="11436" tabRatio="619" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="672" yWindow="636" windowWidth="19836" windowHeight="11436" tabRatio="619" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12290" uniqueCount="4053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12291" uniqueCount="4054">
   <si>
     <t>Field Name</t>
   </si>
@@ -12195,6 +12195,9 @@
   </si>
   <si>
     <t>/productCompanyAllList/?/state</t>
+  </si>
+  <si>
+    <t>Approval_ID</t>
   </si>
 </sst>
 </file>
@@ -12790,8 +12793,8 @@
   <dimension ref="A1:Q1072"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A834" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O846" sqref="O846"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13101,7 +13104,9 @@
         <v>27</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>4053</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
         <v>29</v>
@@ -13115,7 +13120,9 @@
       <c r="N7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="3"/>
+      <c r="O7" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added Type Ahead for Code Value
</commit_message>
<xml_diff>
--- a/substance_dictionary/dictionary_current_all_entities.xlsx
+++ b/substance_dictionary/dictionary_current_all_entities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GSRSFrontend\substance_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67393906-7013-4AA3-8A83-28CB275EBD9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A09809E-D399-4420-82F9-4A41945E4CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="672" yWindow="636" windowWidth="19836" windowHeight="11436" tabRatio="619" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12291" uniqueCount="4054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12292" uniqueCount="4054">
   <si>
     <t>Field Name</t>
   </si>
@@ -12792,9 +12792,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1072"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13318,7 +13318,9 @@
         <v>56</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
updated few features and advanced search
</commit_message>
<xml_diff>
--- a/substance_dictionary/dictionary_current_all_entities.xlsx
+++ b/substance_dictionary/dictionary_current_all_entities.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GSRSFrontend\substance_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A09809E-D399-4420-82F9-4A41945E4CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E924DD3-5B3F-46EB-A01C-7D638FD6D451}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="636" windowWidth="19836" windowHeight="11436" tabRatio="619" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="612" yWindow="36" windowWidth="21480" windowHeight="11880" tabRatio="619" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12292" uniqueCount="4054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12796" uniqueCount="4193">
   <si>
     <t>Field Name</t>
   </si>
@@ -12198,6 +12198,423 @@
   </si>
   <si>
     <t>Approval_ID</t>
+  </si>
+  <si>
+    <t>AdverseEvent</t>
+  </si>
+  <si>
+    <t>AdverseEventPt</t>
+  </si>
+  <si>
+    <t>PT Term</t>
+  </si>
+  <si>
+    <t>AdverseEventCvm</t>
+  </si>
+  <si>
+    <t>/ptTerm</t>
+  </si>
+  <si>
+    <t>root_ptTerm</t>
+  </si>
+  <si>
+    <t>Adverse Event PT PT Term</t>
+  </si>
+  <si>
+    <t>ptTerm</t>
+  </si>
+  <si>
+    <t>Prim SOC</t>
+  </si>
+  <si>
+    <t>/primSoc</t>
+  </si>
+  <si>
+    <t>root_primSoc</t>
+  </si>
+  <si>
+    <t>primSoc</t>
+  </si>
+  <si>
+    <t>Adverse Event PT Prim SOC</t>
+  </si>
+  <si>
+    <t>Case Count</t>
+  </si>
+  <si>
+    <t>SOC Count</t>
+  </si>
+  <si>
+    <t>PT Count</t>
+  </si>
+  <si>
+    <t>PT Count Percent</t>
+  </si>
+  <si>
+    <t>SOC Count Percent</t>
+  </si>
+  <si>
+    <t>PT Count Total Vs Drug</t>
+  </si>
+  <si>
+    <t>PRR</t>
+  </si>
+  <si>
+    <t>Unii/Approval ID</t>
+  </si>
+  <si>
+    <t>Adverse Event PT Deprecated</t>
+  </si>
+  <si>
+    <t>/name</t>
+  </si>
+  <si>
+    <t>root_name</t>
+  </si>
+  <si>
+    <t>/substanceKey</t>
+  </si>
+  <si>
+    <t>root_substanceKey</t>
+  </si>
+  <si>
+    <t>/caseCount</t>
+  </si>
+  <si>
+    <t>root_caseCount</t>
+  </si>
+  <si>
+    <t>ptCount</t>
+  </si>
+  <si>
+    <t>/ptCount</t>
+  </si>
+  <si>
+    <t>/socCount</t>
+  </si>
+  <si>
+    <t>root_socCount</t>
+  </si>
+  <si>
+    <t>caseCount</t>
+  </si>
+  <si>
+    <t>socCount</t>
+  </si>
+  <si>
+    <t>/ptCountPercent</t>
+  </si>
+  <si>
+    <t>root_ptCountPercent</t>
+  </si>
+  <si>
+    <t>ptCountPercent</t>
+  </si>
+  <si>
+    <t>Substance ID</t>
+  </si>
+  <si>
+    <t>UNII/Approval ID</t>
+  </si>
+  <si>
+    <t>/unii</t>
+  </si>
+  <si>
+    <t>/prr</t>
+  </si>
+  <si>
+    <t>root_prr</t>
+  </si>
+  <si>
+    <t>root_unii</t>
+  </si>
+  <si>
+    <t>root_ptCount</t>
+  </si>
+  <si>
+    <t>Adverse Event PT Case Count</t>
+  </si>
+  <si>
+    <t>Adverse Event PT PT Count</t>
+  </si>
+  <si>
+    <t>Adverse Event PT SOC Count</t>
+  </si>
+  <si>
+    <t>Adverse Event PT PRR</t>
+  </si>
+  <si>
+    <t>Adverse Event PT UNII/Approval ID</t>
+  </si>
+  <si>
+    <t>Adverse Event PT Substance Key</t>
+  </si>
+  <si>
+    <t>Adverse Event PT Ingredient Name</t>
+  </si>
+  <si>
+    <t>Adverse Event PT Count Percent</t>
+  </si>
+  <si>
+    <t>Adverse Event PT SOC Count Percent</t>
+  </si>
+  <si>
+    <t>Adverse Event PT Count Total Vs Drug</t>
+  </si>
+  <si>
+    <t>Adverse Event PT Substance ID</t>
+  </si>
+  <si>
+    <t>/socCountPercent</t>
+  </si>
+  <si>
+    <t>/ptCountTotalVsDrug</t>
+  </si>
+  <si>
+    <t>root_ptCountTotalVsDrug</t>
+  </si>
+  <si>
+    <t>ptCountTotalVsDrug</t>
+  </si>
+  <si>
+    <t>root_socCountPercent</t>
+  </si>
+  <si>
+    <t>root_substanceId</t>
+  </si>
+  <si>
+    <t>/substanceId</t>
+  </si>
+  <si>
+    <t>unii</t>
+  </si>
+  <si>
+    <t>substanceId</t>
+  </si>
+  <si>
+    <t>prr</t>
+  </si>
+  <si>
+    <t>socCountPercent</t>
+  </si>
+  <si>
+    <t>PT_TERM</t>
+  </si>
+  <si>
+    <t>Prim_SOC</t>
+  </si>
+  <si>
+    <t>Adverse Event PT ATC Level 1</t>
+  </si>
+  <si>
+    <t>Adverse Event PT ATC Level 2</t>
+  </si>
+  <si>
+    <t>Adverse Event PT ATC Level 3</t>
+  </si>
+  <si>
+    <t>Adverse Event PT ATC Level 4</t>
+  </si>
+  <si>
+    <t>AdverseEventDme</t>
+  </si>
+  <si>
+    <t>root_dmeReactions</t>
+  </si>
+  <si>
+    <t>/dmeReactions</t>
+  </si>
+  <si>
+    <t>DME Reactions</t>
+  </si>
+  <si>
+    <t>dmeReactions</t>
+  </si>
+  <si>
+    <t>DME_Reactions</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Substance ID</t>
+  </si>
+  <si>
+    <t>Adverse Event DME UNII/Approval ID</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Substance Key</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Ingredient Name</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Deprecated</t>
+  </si>
+  <si>
+    <t>Adverse Event DME ATC Level 1</t>
+  </si>
+  <si>
+    <t>PT Term Meddra</t>
+  </si>
+  <si>
+    <t>/ptTermMeddra</t>
+  </si>
+  <si>
+    <t>root_ptTermMeddra</t>
+  </si>
+  <si>
+    <t>ptTermMeddra</t>
+  </si>
+  <si>
+    <t>Adverse Event DME PT Term Meddra</t>
+  </si>
+  <si>
+    <t>PTTerm_Meddra</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Case Count</t>
+  </si>
+  <si>
+    <t>DME Count</t>
+  </si>
+  <si>
+    <t>DME Count Percent</t>
+  </si>
+  <si>
+    <t>Weighted Average PRR</t>
+  </si>
+  <si>
+    <t>Adverse Event DME ATC Level 2</t>
+  </si>
+  <si>
+    <t>Adverse Event DME ATC Level 3</t>
+  </si>
+  <si>
+    <t>Adverse Event DME ATC Level 4</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM ATC Level 1</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM ATC Level 2</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM ATC Level 3</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM ATC Level 4</t>
+  </si>
+  <si>
+    <t>/dmeCount</t>
+  </si>
+  <si>
+    <t>root_dmeCount</t>
+  </si>
+  <si>
+    <t>dmeCount</t>
+  </si>
+  <si>
+    <t>/dmeCountPercent</t>
+  </si>
+  <si>
+    <t>root_dmeCountPercent</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Count</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Count Percent</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Reactions</t>
+  </si>
+  <si>
+    <t>dmeCountPercent</t>
+  </si>
+  <si>
+    <t>/weightedAvgPrr</t>
+  </si>
+  <si>
+    <t>root_weightedAvgPrr</t>
+  </si>
+  <si>
+    <t>Adverse Event DME Weighted Average PRR</t>
+  </si>
+  <si>
+    <t>weightedAvgPrr</t>
+  </si>
+  <si>
+    <t>Adverse Event DME ID</t>
+  </si>
+  <si>
+    <t>/id</t>
+  </si>
+  <si>
+    <t>root_id</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM Deprecated</t>
+  </si>
+  <si>
+    <t>/species</t>
+  </si>
+  <si>
+    <t>root_species</t>
+  </si>
+  <si>
+    <t>Adverse Event CME Species</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>adverseEvent</t>
+  </si>
+  <si>
+    <t>/adverseEvent</t>
+  </si>
+  <si>
+    <t>root_adverseEvent</t>
+  </si>
+  <si>
+    <t>Adverse Event CME Adverse Event</t>
+  </si>
+  <si>
+    <t>Adverse_Event</t>
+  </si>
+  <si>
+    <t>routeOfAdmin</t>
+  </si>
+  <si>
+    <t>/routeOfAdmin</t>
+  </si>
+  <si>
+    <t>root_routeOfAdmin</t>
+  </si>
+  <si>
+    <t>Route_of_Administration</t>
+  </si>
+  <si>
+    <t>Adverse Event CME Route of Administration</t>
+  </si>
+  <si>
+    <t>aeCount</t>
+  </si>
+  <si>
+    <t>/aeCount</t>
+  </si>
+  <si>
+    <t>root_aeCount</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM Substance ID</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM UNII/Approval ID</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM Substance Key</t>
+  </si>
+  <si>
+    <t>Adverse Event CVM Ingredient Name</t>
   </si>
 </sst>
 </file>
@@ -12256,7 +12673,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -12323,6 +12740,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -12336,7 +12771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -12404,6 +12839,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12790,11 +13244,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1072"/>
+  <dimension ref="A1:Q1140"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="B1123" sqref="B1123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -56903,7 +57357,9 @@
       <c r="A1072" s="5" t="s">
         <v>3035</v>
       </c>
-      <c r="B1072" s="5"/>
+      <c r="B1072" s="5" t="s">
+        <v>3035</v>
+      </c>
       <c r="C1072" s="5" t="s">
         <v>82</v>
       </c>
@@ -56914,7 +57370,7 @@
         <v>3010</v>
       </c>
       <c r="F1072" s="5" t="s">
-        <v>4027</v>
+        <v>139</v>
       </c>
       <c r="G1072" s="5" t="s">
         <v>3011</v>
@@ -56934,6 +57390,1971 @@
       </c>
       <c r="O1072" s="5"/>
     </row>
+    <row r="1073" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1073" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1073" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1073" s="29" t="s">
+        <v>4056</v>
+      </c>
+      <c r="D1073" s="29" t="s">
+        <v>4056</v>
+      </c>
+      <c r="E1073" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1073" s="29" t="s">
+        <v>4058</v>
+      </c>
+      <c r="G1073" s="29" t="s">
+        <v>4059</v>
+      </c>
+      <c r="H1073" s="30"/>
+      <c r="I1073" s="29" t="s">
+        <v>4120</v>
+      </c>
+      <c r="J1073" s="30"/>
+      <c r="K1073" s="29" t="s">
+        <v>4060</v>
+      </c>
+      <c r="L1073" s="29" t="s">
+        <v>4061</v>
+      </c>
+      <c r="M1073" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1073" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1073" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1073" s="30"/>
+      <c r="Q1073" s="30"/>
+    </row>
+    <row r="1074" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1074" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1074" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1074" s="29" t="s">
+        <v>4062</v>
+      </c>
+      <c r="D1074" s="29" t="s">
+        <v>4062</v>
+      </c>
+      <c r="E1074" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1074" s="29" t="s">
+        <v>4063</v>
+      </c>
+      <c r="G1074" s="29" t="s">
+        <v>4064</v>
+      </c>
+      <c r="H1074" s="30"/>
+      <c r="I1074" s="29" t="s">
+        <v>4121</v>
+      </c>
+      <c r="J1074" s="30"/>
+      <c r="K1074" s="29" t="s">
+        <v>4066</v>
+      </c>
+      <c r="L1074" s="29" t="s">
+        <v>4065</v>
+      </c>
+      <c r="M1074" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1074" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1074" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1074" s="30"/>
+      <c r="Q1074" s="30"/>
+    </row>
+    <row r="1075" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1075" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1075" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1075" s="29" t="s">
+        <v>4067</v>
+      </c>
+      <c r="D1075" s="29" t="s">
+        <v>4067</v>
+      </c>
+      <c r="E1075" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1075" s="29" t="s">
+        <v>4080</v>
+      </c>
+      <c r="G1075" s="29" t="s">
+        <v>4081</v>
+      </c>
+      <c r="H1075" s="30"/>
+      <c r="I1075" s="30"/>
+      <c r="J1075" s="30"/>
+      <c r="K1075" s="29" t="s">
+        <v>4098</v>
+      </c>
+      <c r="L1075" s="29" t="s">
+        <v>4086</v>
+      </c>
+      <c r="M1075" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1075" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1075" s="29"/>
+      <c r="P1075" s="30"/>
+      <c r="Q1075" s="30"/>
+    </row>
+    <row r="1076" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1076" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1076" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1076" s="29" t="s">
+        <v>4069</v>
+      </c>
+      <c r="D1076" s="29" t="s">
+        <v>4069</v>
+      </c>
+      <c r="E1076" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1076" s="29" t="s">
+        <v>4083</v>
+      </c>
+      <c r="G1076" s="29" t="s">
+        <v>4097</v>
+      </c>
+      <c r="H1076" s="30"/>
+      <c r="I1076" s="30"/>
+      <c r="J1076" s="30"/>
+      <c r="K1076" s="29" t="s">
+        <v>4099</v>
+      </c>
+      <c r="L1076" s="29" t="s">
+        <v>4082</v>
+      </c>
+      <c r="M1076" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1076" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1076" s="29"/>
+      <c r="P1076" s="30"/>
+      <c r="Q1076" s="30"/>
+    </row>
+    <row r="1077" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1077" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1077" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1077" s="29" t="s">
+        <v>4068</v>
+      </c>
+      <c r="D1077" s="29" t="s">
+        <v>4068</v>
+      </c>
+      <c r="E1077" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1077" s="29" t="s">
+        <v>4084</v>
+      </c>
+      <c r="G1077" s="29" t="s">
+        <v>4085</v>
+      </c>
+      <c r="H1077" s="30"/>
+      <c r="I1077" s="30"/>
+      <c r="J1077" s="30"/>
+      <c r="K1077" s="29" t="s">
+        <v>4100</v>
+      </c>
+      <c r="L1077" s="29" t="s">
+        <v>4087</v>
+      </c>
+      <c r="M1077" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1077" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1077" s="29"/>
+      <c r="P1077" s="30"/>
+      <c r="Q1077" s="30"/>
+    </row>
+    <row r="1078" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1078" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1078" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1078" s="29" t="s">
+        <v>4070</v>
+      </c>
+      <c r="D1078" s="29" t="s">
+        <v>4070</v>
+      </c>
+      <c r="E1078" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1078" s="29" t="s">
+        <v>4088</v>
+      </c>
+      <c r="G1078" s="29" t="s">
+        <v>4089</v>
+      </c>
+      <c r="H1078" s="30"/>
+      <c r="I1078" s="30"/>
+      <c r="J1078" s="30"/>
+      <c r="K1078" s="29" t="s">
+        <v>4105</v>
+      </c>
+      <c r="L1078" s="29" t="s">
+        <v>4090</v>
+      </c>
+      <c r="M1078" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1078" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1078" s="29"/>
+      <c r="P1078" s="30"/>
+      <c r="Q1078" s="30"/>
+    </row>
+    <row r="1079" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1079" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1079" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1079" s="29" t="s">
+        <v>4071</v>
+      </c>
+      <c r="D1079" s="29" t="s">
+        <v>4071</v>
+      </c>
+      <c r="E1079" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1079" s="29" t="s">
+        <v>4109</v>
+      </c>
+      <c r="G1079" s="29" t="s">
+        <v>4113</v>
+      </c>
+      <c r="H1079" s="30"/>
+      <c r="I1079" s="30"/>
+      <c r="J1079" s="30"/>
+      <c r="K1079" s="29" t="s">
+        <v>4106</v>
+      </c>
+      <c r="L1079" s="29" t="s">
+        <v>4119</v>
+      </c>
+      <c r="M1079" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1079" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1079" s="29"/>
+      <c r="P1079" s="30"/>
+      <c r="Q1079" s="30"/>
+    </row>
+    <row r="1080" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1080" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1080" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1080" s="29" t="s">
+        <v>4072</v>
+      </c>
+      <c r="D1080" s="29" t="s">
+        <v>4072</v>
+      </c>
+      <c r="E1080" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1080" s="29" t="s">
+        <v>4110</v>
+      </c>
+      <c r="G1080" s="29" t="s">
+        <v>4111</v>
+      </c>
+      <c r="H1080" s="30"/>
+      <c r="I1080" s="30"/>
+      <c r="J1080" s="30"/>
+      <c r="K1080" s="29" t="s">
+        <v>4107</v>
+      </c>
+      <c r="L1080" s="29" t="s">
+        <v>4112</v>
+      </c>
+      <c r="M1080" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1080" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1080" s="29"/>
+      <c r="P1080" s="30"/>
+      <c r="Q1080" s="30"/>
+    </row>
+    <row r="1081" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1081" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1081" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1081" s="29" t="s">
+        <v>4073</v>
+      </c>
+      <c r="D1081" s="29" t="s">
+        <v>4073</v>
+      </c>
+      <c r="E1081" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1081" s="29" t="s">
+        <v>4094</v>
+      </c>
+      <c r="G1081" s="29" t="s">
+        <v>4095</v>
+      </c>
+      <c r="H1081" s="30"/>
+      <c r="I1081" s="30"/>
+      <c r="J1081" s="30"/>
+      <c r="K1081" s="29" t="s">
+        <v>4101</v>
+      </c>
+      <c r="L1081" s="29" t="s">
+        <v>4118</v>
+      </c>
+      <c r="M1081" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1081" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1081" s="29"/>
+      <c r="P1081" s="30"/>
+      <c r="Q1081" s="30"/>
+    </row>
+    <row r="1082" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1082" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1082" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1082" s="29" t="s">
+        <v>4091</v>
+      </c>
+      <c r="D1082" s="29" t="s">
+        <v>4091</v>
+      </c>
+      <c r="E1082" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1082" s="29" t="s">
+        <v>4115</v>
+      </c>
+      <c r="G1082" s="29" t="s">
+        <v>4114</v>
+      </c>
+      <c r="H1082" s="30"/>
+      <c r="I1082" s="30"/>
+      <c r="J1082" s="30"/>
+      <c r="K1082" s="29" t="s">
+        <v>4108</v>
+      </c>
+      <c r="L1082" s="29" t="s">
+        <v>4117</v>
+      </c>
+      <c r="M1082" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1082" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1082" s="29"/>
+      <c r="P1082" s="30"/>
+      <c r="Q1082" s="30"/>
+    </row>
+    <row r="1083" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1083" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1083" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1083" s="29" t="s">
+        <v>4092</v>
+      </c>
+      <c r="D1083" s="29" t="s">
+        <v>4074</v>
+      </c>
+      <c r="E1083" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1083" s="29" t="s">
+        <v>4093</v>
+      </c>
+      <c r="G1083" s="29" t="s">
+        <v>4096</v>
+      </c>
+      <c r="H1083" s="30"/>
+      <c r="I1083" s="30"/>
+      <c r="J1083" s="30"/>
+      <c r="K1083" s="29" t="s">
+        <v>4102</v>
+      </c>
+      <c r="L1083" s="29" t="s">
+        <v>4116</v>
+      </c>
+      <c r="M1083" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1083" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1083" s="29"/>
+      <c r="P1083" s="30"/>
+      <c r="Q1083" s="30"/>
+    </row>
+    <row r="1084" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1084" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1084" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1084" s="29" t="s">
+        <v>2741</v>
+      </c>
+      <c r="D1084" s="29" t="s">
+        <v>2741</v>
+      </c>
+      <c r="E1084" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1084" s="29" t="s">
+        <v>4078</v>
+      </c>
+      <c r="G1084" s="29" t="s">
+        <v>4079</v>
+      </c>
+      <c r="H1084" s="30"/>
+      <c r="I1084" s="30"/>
+      <c r="J1084" s="30"/>
+      <c r="K1084" s="29" t="s">
+        <v>4103</v>
+      </c>
+      <c r="L1084" s="29" t="s">
+        <v>2986</v>
+      </c>
+      <c r="M1084" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1084" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1084" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1084" s="30"/>
+      <c r="Q1084" s="30"/>
+    </row>
+    <row r="1085" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1085" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1085" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1085" s="29" t="s">
+        <v>2756</v>
+      </c>
+      <c r="D1085" s="29" t="s">
+        <v>2756</v>
+      </c>
+      <c r="E1085" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1085" s="29" t="s">
+        <v>4076</v>
+      </c>
+      <c r="G1085" s="29" t="s">
+        <v>4077</v>
+      </c>
+      <c r="H1085" s="30"/>
+      <c r="I1085" s="29" t="s">
+        <v>3406</v>
+      </c>
+      <c r="J1085" s="30"/>
+      <c r="K1085" s="29" t="s">
+        <v>4104</v>
+      </c>
+      <c r="L1085" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1085" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1085" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1085" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1085" s="30"/>
+      <c r="Q1085" s="30"/>
+    </row>
+    <row r="1086" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1086" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1086" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1086" s="29" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D1086" s="29" t="s">
+        <v>4075</v>
+      </c>
+      <c r="E1086" s="29" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1086" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1086" s="29" t="s">
+        <v>3011</v>
+      </c>
+      <c r="H1086" s="30"/>
+      <c r="I1086" s="30"/>
+      <c r="J1086" s="30"/>
+      <c r="K1086" s="29" t="s">
+        <v>4075</v>
+      </c>
+      <c r="L1086" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1086" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1086" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1086" s="29"/>
+      <c r="P1086" s="30"/>
+      <c r="Q1086" s="30"/>
+    </row>
+    <row r="1087" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1087" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1087" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1087" s="29" t="s">
+        <v>4122</v>
+      </c>
+      <c r="D1087" s="29" t="s">
+        <v>4122</v>
+      </c>
+      <c r="E1087" s="29" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1087" s="29"/>
+      <c r="G1087" s="29"/>
+      <c r="H1087" s="30"/>
+      <c r="I1087" s="30"/>
+      <c r="J1087" s="30"/>
+      <c r="K1087" s="29" t="s">
+        <v>4122</v>
+      </c>
+      <c r="L1087" s="29"/>
+      <c r="M1087" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1087" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1087" s="29"/>
+      <c r="P1087" s="30"/>
+      <c r="Q1087" s="30"/>
+    </row>
+    <row r="1088" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1088" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1088" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1088" s="29" t="s">
+        <v>4123</v>
+      </c>
+      <c r="D1088" s="29" t="s">
+        <v>4123</v>
+      </c>
+      <c r="E1088" s="29" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1088" s="29"/>
+      <c r="G1088" s="29"/>
+      <c r="H1088" s="30"/>
+      <c r="I1088" s="30"/>
+      <c r="J1088" s="30"/>
+      <c r="K1088" s="29" t="s">
+        <v>4123</v>
+      </c>
+      <c r="L1088" s="29"/>
+      <c r="M1088" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1088" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1088" s="29"/>
+      <c r="P1088" s="30"/>
+      <c r="Q1088" s="30"/>
+    </row>
+    <row r="1089" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1089" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1089" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1089" s="29" t="s">
+        <v>4124</v>
+      </c>
+      <c r="D1089" s="29" t="s">
+        <v>4124</v>
+      </c>
+      <c r="E1089" s="29" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1089" s="29"/>
+      <c r="G1089" s="29"/>
+      <c r="H1089" s="30"/>
+      <c r="I1089" s="30"/>
+      <c r="J1089" s="30"/>
+      <c r="K1089" s="29" t="s">
+        <v>4124</v>
+      </c>
+      <c r="L1089" s="29"/>
+      <c r="M1089" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1089" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1089" s="29"/>
+      <c r="P1089" s="30"/>
+      <c r="Q1089" s="30"/>
+    </row>
+    <row r="1090" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1090" s="29" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1090" s="29" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1090" s="29" t="s">
+        <v>4125</v>
+      </c>
+      <c r="D1090" s="29" t="s">
+        <v>4125</v>
+      </c>
+      <c r="E1090" s="29" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1090" s="29"/>
+      <c r="G1090" s="29"/>
+      <c r="H1090" s="30"/>
+      <c r="I1090" s="30"/>
+      <c r="J1090" s="30"/>
+      <c r="K1090" s="29" t="s">
+        <v>4125</v>
+      </c>
+      <c r="L1090" s="29"/>
+      <c r="M1090" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1090" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1090" s="29"/>
+      <c r="P1090" s="31"/>
+      <c r="Q1090" s="31"/>
+    </row>
+    <row r="1091" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1091" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1091" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1091" s="32" t="s">
+        <v>4168</v>
+      </c>
+      <c r="D1091" s="32" t="s">
+        <v>4168</v>
+      </c>
+      <c r="E1091" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1091" s="32" t="s">
+        <v>4169</v>
+      </c>
+      <c r="G1091" s="32" t="s">
+        <v>4170</v>
+      </c>
+      <c r="H1091" s="33"/>
+      <c r="I1091" s="32"/>
+      <c r="J1091" s="33"/>
+      <c r="K1091" s="32" t="s">
+        <v>4168</v>
+      </c>
+      <c r="L1091" s="32" t="s">
+        <v>894</v>
+      </c>
+      <c r="M1091" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1091" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1091" s="32"/>
+      <c r="P1091" s="34"/>
+      <c r="Q1091" s="34"/>
+    </row>
+    <row r="1092" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1092" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1092" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1092" s="32" t="s">
+        <v>4129</v>
+      </c>
+      <c r="D1092" s="32" t="s">
+        <v>4129</v>
+      </c>
+      <c r="E1092" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1092" s="32" t="s">
+        <v>4128</v>
+      </c>
+      <c r="G1092" s="32" t="s">
+        <v>4127</v>
+      </c>
+      <c r="H1092" s="33"/>
+      <c r="I1092" s="32" t="s">
+        <v>4131</v>
+      </c>
+      <c r="J1092" s="33"/>
+      <c r="K1092" s="32" t="s">
+        <v>4162</v>
+      </c>
+      <c r="L1092" s="32" t="s">
+        <v>4130</v>
+      </c>
+      <c r="M1092" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1092" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1092" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1092" s="34"/>
+      <c r="Q1092" s="34"/>
+    </row>
+    <row r="1093" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1093" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1093" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1093" s="32" t="s">
+        <v>4138</v>
+      </c>
+      <c r="D1093" s="32" t="s">
+        <v>4138</v>
+      </c>
+      <c r="E1093" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1093" s="32" t="s">
+        <v>4139</v>
+      </c>
+      <c r="G1093" s="32" t="s">
+        <v>4140</v>
+      </c>
+      <c r="H1093" s="33"/>
+      <c r="I1093" s="32" t="s">
+        <v>4143</v>
+      </c>
+      <c r="J1093" s="33"/>
+      <c r="K1093" s="32" t="s">
+        <v>4142</v>
+      </c>
+      <c r="L1093" s="32" t="s">
+        <v>4141</v>
+      </c>
+      <c r="M1093" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1093" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1093" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1093" s="34"/>
+      <c r="Q1093" s="34"/>
+    </row>
+    <row r="1094" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1094" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1094" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1094" s="32" t="s">
+        <v>4067</v>
+      </c>
+      <c r="D1094" s="32" t="s">
+        <v>4067</v>
+      </c>
+      <c r="E1094" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1094" s="32" t="s">
+        <v>4080</v>
+      </c>
+      <c r="G1094" s="32" t="s">
+        <v>4081</v>
+      </c>
+      <c r="H1094" s="33"/>
+      <c r="I1094" s="32"/>
+      <c r="J1094" s="33"/>
+      <c r="K1094" s="32" t="s">
+        <v>4144</v>
+      </c>
+      <c r="L1094" s="32" t="s">
+        <v>4086</v>
+      </c>
+      <c r="M1094" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1094" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1094" s="32"/>
+      <c r="P1094" s="34"/>
+      <c r="Q1094" s="34"/>
+    </row>
+    <row r="1095" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1095" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1095" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1095" s="32" t="s">
+        <v>4145</v>
+      </c>
+      <c r="D1095" s="32" t="s">
+        <v>4145</v>
+      </c>
+      <c r="E1095" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1095" s="32" t="s">
+        <v>4155</v>
+      </c>
+      <c r="G1095" s="32" t="s">
+        <v>4156</v>
+      </c>
+      <c r="H1095" s="33"/>
+      <c r="I1095" s="32"/>
+      <c r="J1095" s="33"/>
+      <c r="K1095" s="32" t="s">
+        <v>4160</v>
+      </c>
+      <c r="L1095" s="32" t="s">
+        <v>4157</v>
+      </c>
+      <c r="M1095" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1095" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1095" s="32"/>
+      <c r="P1095" s="34"/>
+      <c r="Q1095" s="34"/>
+    </row>
+    <row r="1096" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1096" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1096" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1096" s="32" t="s">
+        <v>4146</v>
+      </c>
+      <c r="D1096" s="32" t="s">
+        <v>4146</v>
+      </c>
+      <c r="E1096" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1096" s="32" t="s">
+        <v>4158</v>
+      </c>
+      <c r="G1096" s="32" t="s">
+        <v>4159</v>
+      </c>
+      <c r="H1096" s="33"/>
+      <c r="I1096" s="32"/>
+      <c r="J1096" s="33"/>
+      <c r="K1096" s="32" t="s">
+        <v>4161</v>
+      </c>
+      <c r="L1096" s="32" t="s">
+        <v>4163</v>
+      </c>
+      <c r="M1096" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1096" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1096" s="32"/>
+      <c r="P1096" s="34"/>
+      <c r="Q1096" s="34"/>
+    </row>
+    <row r="1097" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1097" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1097" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1097" s="32" t="s">
+        <v>4147</v>
+      </c>
+      <c r="D1097" s="32" t="s">
+        <v>4147</v>
+      </c>
+      <c r="E1097" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1097" s="32" t="s">
+        <v>4164</v>
+      </c>
+      <c r="G1097" s="32" t="s">
+        <v>4165</v>
+      </c>
+      <c r="H1097" s="33"/>
+      <c r="I1097" s="32"/>
+      <c r="J1097" s="33"/>
+      <c r="K1097" s="32" t="s">
+        <v>4166</v>
+      </c>
+      <c r="L1097" s="32" t="s">
+        <v>4167</v>
+      </c>
+      <c r="M1097" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1097" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1097" s="32"/>
+      <c r="P1097" s="34"/>
+      <c r="Q1097" s="34"/>
+    </row>
+    <row r="1098" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1098" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1098" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1098" s="32" t="s">
+        <v>4091</v>
+      </c>
+      <c r="D1098" s="32" t="s">
+        <v>4091</v>
+      </c>
+      <c r="E1098" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1098" s="32" t="s">
+        <v>4115</v>
+      </c>
+      <c r="G1098" s="32" t="s">
+        <v>4114</v>
+      </c>
+      <c r="H1098" s="33"/>
+      <c r="I1098" s="32"/>
+      <c r="J1098" s="33"/>
+      <c r="K1098" s="32" t="s">
+        <v>4132</v>
+      </c>
+      <c r="L1098" s="32" t="s">
+        <v>4117</v>
+      </c>
+      <c r="M1098" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1098" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1098" s="32"/>
+      <c r="P1098" s="34"/>
+      <c r="Q1098" s="34"/>
+    </row>
+    <row r="1099" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1099" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1099" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1099" s="32" t="s">
+        <v>4092</v>
+      </c>
+      <c r="D1099" s="32" t="s">
+        <v>4074</v>
+      </c>
+      <c r="E1099" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1099" s="32" t="s">
+        <v>4093</v>
+      </c>
+      <c r="G1099" s="32" t="s">
+        <v>4096</v>
+      </c>
+      <c r="H1099" s="33"/>
+      <c r="I1099" s="32"/>
+      <c r="J1099" s="33"/>
+      <c r="K1099" s="32" t="s">
+        <v>4133</v>
+      </c>
+      <c r="L1099" s="32" t="s">
+        <v>4116</v>
+      </c>
+      <c r="M1099" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1099" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1099" s="32"/>
+      <c r="P1099" s="34"/>
+      <c r="Q1099" s="34"/>
+    </row>
+    <row r="1100" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1100" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1100" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1100" s="32" t="s">
+        <v>2741</v>
+      </c>
+      <c r="D1100" s="32" t="s">
+        <v>2741</v>
+      </c>
+      <c r="E1100" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1100" s="32" t="s">
+        <v>4078</v>
+      </c>
+      <c r="G1100" s="32" t="s">
+        <v>4079</v>
+      </c>
+      <c r="H1100" s="33"/>
+      <c r="I1100" s="32"/>
+      <c r="J1100" s="33"/>
+      <c r="K1100" s="32" t="s">
+        <v>4134</v>
+      </c>
+      <c r="L1100" s="32" t="s">
+        <v>2986</v>
+      </c>
+      <c r="M1100" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1100" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1100" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1100" s="34"/>
+      <c r="Q1100" s="34"/>
+    </row>
+    <row r="1101" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1101" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1101" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1101" s="32" t="s">
+        <v>2756</v>
+      </c>
+      <c r="D1101" s="32" t="s">
+        <v>2756</v>
+      </c>
+      <c r="E1101" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1101" s="32" t="s">
+        <v>4076</v>
+      </c>
+      <c r="G1101" s="32" t="s">
+        <v>4077</v>
+      </c>
+      <c r="H1101" s="33"/>
+      <c r="I1101" s="32" t="s">
+        <v>3406</v>
+      </c>
+      <c r="J1101" s="33"/>
+      <c r="K1101" s="32" t="s">
+        <v>4135</v>
+      </c>
+      <c r="L1101" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1101" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1101" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1101" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1101" s="34"/>
+      <c r="Q1101" s="34"/>
+    </row>
+    <row r="1102" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1102" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1102" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1102" s="32" t="s">
+        <v>4136</v>
+      </c>
+      <c r="D1102" s="32" t="s">
+        <v>4136</v>
+      </c>
+      <c r="E1102" s="32" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1102" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1102" s="32" t="s">
+        <v>3011</v>
+      </c>
+      <c r="H1102" s="33"/>
+      <c r="I1102" s="33"/>
+      <c r="J1102" s="33"/>
+      <c r="K1102" s="32" t="s">
+        <v>4075</v>
+      </c>
+      <c r="L1102" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1102" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1102" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1102" s="32"/>
+      <c r="P1102" s="34"/>
+      <c r="Q1102" s="34"/>
+    </row>
+    <row r="1103" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1103" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1103" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1103" s="32" t="s">
+        <v>4137</v>
+      </c>
+      <c r="D1103" s="32" t="s">
+        <v>4137</v>
+      </c>
+      <c r="E1103" s="32" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1103" s="32"/>
+      <c r="G1103" s="32"/>
+      <c r="H1103" s="33"/>
+      <c r="I1103" s="32"/>
+      <c r="J1103" s="33"/>
+      <c r="K1103" s="32" t="s">
+        <v>4137</v>
+      </c>
+      <c r="L1103" s="32"/>
+      <c r="M1103" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1103" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1103" s="32"/>
+      <c r="P1103" s="34"/>
+      <c r="Q1103" s="34"/>
+    </row>
+    <row r="1104" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1104" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1104" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1104" s="32" t="s">
+        <v>4148</v>
+      </c>
+      <c r="D1104" s="32" t="s">
+        <v>4148</v>
+      </c>
+      <c r="E1104" s="32" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1104" s="32"/>
+      <c r="G1104" s="32"/>
+      <c r="H1104" s="33"/>
+      <c r="I1104" s="32"/>
+      <c r="J1104" s="33"/>
+      <c r="K1104" s="32" t="s">
+        <v>4148</v>
+      </c>
+      <c r="L1104" s="32"/>
+      <c r="M1104" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1104" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1104" s="32"/>
+      <c r="P1104" s="34"/>
+      <c r="Q1104" s="34"/>
+    </row>
+    <row r="1105" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1105" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1105" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1105" s="32" t="s">
+        <v>4149</v>
+      </c>
+      <c r="D1105" s="32" t="s">
+        <v>4149</v>
+      </c>
+      <c r="E1105" s="32" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1105" s="32"/>
+      <c r="G1105" s="32"/>
+      <c r="H1105" s="33"/>
+      <c r="I1105" s="32"/>
+      <c r="J1105" s="33"/>
+      <c r="K1105" s="32" t="s">
+        <v>4149</v>
+      </c>
+      <c r="L1105" s="32"/>
+      <c r="M1105" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1105" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1105" s="32"/>
+      <c r="P1105" s="34"/>
+      <c r="Q1105" s="34"/>
+    </row>
+    <row r="1106" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1106" s="32" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1106" s="32" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C1106" s="32" t="s">
+        <v>4150</v>
+      </c>
+      <c r="D1106" s="32" t="s">
+        <v>4150</v>
+      </c>
+      <c r="E1106" s="32" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1106" s="32"/>
+      <c r="G1106" s="32"/>
+      <c r="H1106" s="33"/>
+      <c r="I1106" s="32"/>
+      <c r="J1106" s="33"/>
+      <c r="K1106" s="32" t="s">
+        <v>4150</v>
+      </c>
+      <c r="L1106" s="32"/>
+      <c r="M1106" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1106" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1106" s="32"/>
+      <c r="P1106" s="34"/>
+      <c r="Q1106" s="34"/>
+    </row>
+    <row r="1107" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1107" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1107" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1107" s="35" t="s">
+        <v>2534</v>
+      </c>
+      <c r="D1107" s="35" t="s">
+        <v>4175</v>
+      </c>
+      <c r="E1107" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1107" s="35" t="s">
+        <v>4172</v>
+      </c>
+      <c r="G1107" s="35" t="s">
+        <v>4173</v>
+      </c>
+      <c r="H1107" s="36"/>
+      <c r="I1107" s="35" t="s">
+        <v>2534</v>
+      </c>
+      <c r="J1107" s="36"/>
+      <c r="K1107" s="35" t="s">
+        <v>4174</v>
+      </c>
+      <c r="L1107" s="35" t="s">
+        <v>4175</v>
+      </c>
+      <c r="M1107" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1107" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1107" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1107" s="37"/>
+      <c r="Q1107" s="37"/>
+    </row>
+    <row r="1108" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1108" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1108" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1108" s="35" t="s">
+        <v>4176</v>
+      </c>
+      <c r="D1108" s="35" t="s">
+        <v>4176</v>
+      </c>
+      <c r="E1108" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1108" s="35" t="s">
+        <v>4177</v>
+      </c>
+      <c r="G1108" s="35" t="s">
+        <v>4178</v>
+      </c>
+      <c r="H1108" s="36"/>
+      <c r="I1108" s="35" t="s">
+        <v>4180</v>
+      </c>
+      <c r="J1108" s="36"/>
+      <c r="K1108" s="35" t="s">
+        <v>4179</v>
+      </c>
+      <c r="L1108" s="35" t="s">
+        <v>4176</v>
+      </c>
+      <c r="M1108" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1108" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1108" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1108" s="37"/>
+      <c r="Q1108" s="37"/>
+    </row>
+    <row r="1109" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1109" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1109" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1109" s="35" t="s">
+        <v>4181</v>
+      </c>
+      <c r="D1109" s="35" t="s">
+        <v>4181</v>
+      </c>
+      <c r="E1109" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1109" s="35" t="s">
+        <v>4182</v>
+      </c>
+      <c r="G1109" s="35" t="s">
+        <v>4183</v>
+      </c>
+      <c r="H1109" s="36"/>
+      <c r="I1109" s="35" t="s">
+        <v>4184</v>
+      </c>
+      <c r="J1109" s="36"/>
+      <c r="K1109" s="35" t="s">
+        <v>4185</v>
+      </c>
+      <c r="L1109" s="35" t="s">
+        <v>4181</v>
+      </c>
+      <c r="M1109" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1109" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1109" s="35"/>
+      <c r="P1109" s="37"/>
+      <c r="Q1109" s="37"/>
+    </row>
+    <row r="1110" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1110" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1110" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1110" s="35" t="s">
+        <v>4181</v>
+      </c>
+      <c r="D1110" s="35" t="s">
+        <v>4181</v>
+      </c>
+      <c r="E1110" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1110" s="35" t="s">
+        <v>4182</v>
+      </c>
+      <c r="G1110" s="35" t="s">
+        <v>4183</v>
+      </c>
+      <c r="H1110" s="36"/>
+      <c r="I1110" s="35" t="s">
+        <v>4184</v>
+      </c>
+      <c r="J1110" s="36"/>
+      <c r="K1110" s="35" t="s">
+        <v>4185</v>
+      </c>
+      <c r="L1110" s="35" t="s">
+        <v>4181</v>
+      </c>
+      <c r="M1110" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1110" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1110" s="35"/>
+      <c r="P1110" s="37"/>
+      <c r="Q1110" s="37"/>
+    </row>
+    <row r="1111" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1111" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1111" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1111" s="35" t="s">
+        <v>4186</v>
+      </c>
+      <c r="D1111" s="35" t="s">
+        <v>4186</v>
+      </c>
+      <c r="E1111" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1111" s="35" t="s">
+        <v>4187</v>
+      </c>
+      <c r="G1111" s="35" t="s">
+        <v>4188</v>
+      </c>
+      <c r="H1111" s="36"/>
+      <c r="I1111" s="35"/>
+      <c r="J1111" s="36"/>
+      <c r="K1111" s="35" t="s">
+        <v>4185</v>
+      </c>
+      <c r="L1111" s="35" t="s">
+        <v>4186</v>
+      </c>
+      <c r="M1111" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1111" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1111" s="35"/>
+      <c r="P1111" s="37"/>
+      <c r="Q1111" s="37"/>
+    </row>
+    <row r="1112" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1112" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1112" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1112" s="35" t="s">
+        <v>4091</v>
+      </c>
+      <c r="D1112" s="35" t="s">
+        <v>4091</v>
+      </c>
+      <c r="E1112" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1112" s="35" t="s">
+        <v>4115</v>
+      </c>
+      <c r="G1112" s="35" t="s">
+        <v>4114</v>
+      </c>
+      <c r="H1112" s="36"/>
+      <c r="I1112" s="35"/>
+      <c r="J1112" s="36"/>
+      <c r="K1112" s="35" t="s">
+        <v>4189</v>
+      </c>
+      <c r="L1112" s="35" t="s">
+        <v>4117</v>
+      </c>
+      <c r="M1112" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1112" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1112" s="35"/>
+      <c r="P1112" s="37"/>
+      <c r="Q1112" s="37"/>
+    </row>
+    <row r="1113" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1113" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1113" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1113" s="35" t="s">
+        <v>4092</v>
+      </c>
+      <c r="D1113" s="35" t="s">
+        <v>4074</v>
+      </c>
+      <c r="E1113" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1113" s="35" t="s">
+        <v>4093</v>
+      </c>
+      <c r="G1113" s="35" t="s">
+        <v>4096</v>
+      </c>
+      <c r="H1113" s="36"/>
+      <c r="I1113" s="35"/>
+      <c r="J1113" s="36"/>
+      <c r="K1113" s="35" t="s">
+        <v>4190</v>
+      </c>
+      <c r="L1113" s="35" t="s">
+        <v>4116</v>
+      </c>
+      <c r="M1113" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1113" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1113" s="35"/>
+      <c r="P1113" s="37"/>
+      <c r="Q1113" s="37"/>
+    </row>
+    <row r="1114" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1114" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1114" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1114" s="35" t="s">
+        <v>2741</v>
+      </c>
+      <c r="D1114" s="35" t="s">
+        <v>2741</v>
+      </c>
+      <c r="E1114" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1114" s="35" t="s">
+        <v>4078</v>
+      </c>
+      <c r="G1114" s="35" t="s">
+        <v>4079</v>
+      </c>
+      <c r="H1114" s="36"/>
+      <c r="I1114" s="35"/>
+      <c r="J1114" s="36"/>
+      <c r="K1114" s="35" t="s">
+        <v>4191</v>
+      </c>
+      <c r="L1114" s="35" t="s">
+        <v>2986</v>
+      </c>
+      <c r="M1114" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1114" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1114" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1114" s="37"/>
+      <c r="Q1114" s="37"/>
+    </row>
+    <row r="1115" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1115" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1115" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1115" s="35" t="s">
+        <v>2756</v>
+      </c>
+      <c r="D1115" s="35" t="s">
+        <v>2756</v>
+      </c>
+      <c r="E1115" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1115" s="35" t="s">
+        <v>4076</v>
+      </c>
+      <c r="G1115" s="35" t="s">
+        <v>4077</v>
+      </c>
+      <c r="H1115" s="36"/>
+      <c r="I1115" s="35" t="s">
+        <v>3406</v>
+      </c>
+      <c r="J1115" s="36"/>
+      <c r="K1115" s="35" t="s">
+        <v>4192</v>
+      </c>
+      <c r="L1115" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1115" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1115" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1115" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1115" s="37"/>
+      <c r="Q1115" s="37"/>
+    </row>
+    <row r="1116" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1116" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1116" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1116" s="35" t="s">
+        <v>4171</v>
+      </c>
+      <c r="D1116" s="35" t="s">
+        <v>4171</v>
+      </c>
+      <c r="E1116" s="35" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1116" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1116" s="35" t="s">
+        <v>3011</v>
+      </c>
+      <c r="H1116" s="36"/>
+      <c r="I1116" s="36"/>
+      <c r="J1116" s="36"/>
+      <c r="K1116" s="35" t="s">
+        <v>4171</v>
+      </c>
+      <c r="L1116" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1116" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1116" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1116" s="36"/>
+      <c r="P1116" s="37"/>
+      <c r="Q1116" s="37"/>
+    </row>
+    <row r="1117" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1117" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1117" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1117" s="35" t="s">
+        <v>4151</v>
+      </c>
+      <c r="D1117" s="35" t="s">
+        <v>4151</v>
+      </c>
+      <c r="E1117" s="35" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1117" s="36"/>
+      <c r="G1117" s="36"/>
+      <c r="H1117" s="36"/>
+      <c r="I1117" s="36"/>
+      <c r="J1117" s="36"/>
+      <c r="K1117" s="35" t="s">
+        <v>4151</v>
+      </c>
+      <c r="L1117" s="36"/>
+      <c r="M1117" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1117" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1117" s="36"/>
+      <c r="P1117" s="36"/>
+      <c r="Q1117" s="36"/>
+    </row>
+    <row r="1118" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1118" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1118" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1118" s="35" t="s">
+        <v>4152</v>
+      </c>
+      <c r="D1118" s="35" t="s">
+        <v>4152</v>
+      </c>
+      <c r="E1118" s="35" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1118" s="36"/>
+      <c r="G1118" s="36"/>
+      <c r="H1118" s="36"/>
+      <c r="I1118" s="36"/>
+      <c r="J1118" s="36"/>
+      <c r="K1118" s="35" t="s">
+        <v>4152</v>
+      </c>
+      <c r="L1118" s="36"/>
+      <c r="M1118" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1118" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1118" s="36"/>
+      <c r="P1118" s="36"/>
+      <c r="Q1118" s="36"/>
+    </row>
+    <row r="1119" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1119" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1119" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1119" s="35" t="s">
+        <v>4153</v>
+      </c>
+      <c r="D1119" s="35" t="s">
+        <v>4153</v>
+      </c>
+      <c r="E1119" s="35" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1119" s="36"/>
+      <c r="G1119" s="36"/>
+      <c r="H1119" s="36"/>
+      <c r="I1119" s="36"/>
+      <c r="J1119" s="36"/>
+      <c r="K1119" s="35" t="s">
+        <v>4153</v>
+      </c>
+      <c r="L1119" s="36"/>
+      <c r="M1119" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1119" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1119" s="36"/>
+      <c r="P1119" s="36"/>
+      <c r="Q1119" s="36"/>
+    </row>
+    <row r="1120" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1120" s="35" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B1120" s="35" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C1120" s="35" t="s">
+        <v>4154</v>
+      </c>
+      <c r="D1120" s="35" t="s">
+        <v>4154</v>
+      </c>
+      <c r="E1120" s="35" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1120" s="36"/>
+      <c r="G1120" s="36"/>
+      <c r="H1120" s="36"/>
+      <c r="I1120" s="36"/>
+      <c r="J1120" s="36"/>
+      <c r="K1120" s="35" t="s">
+        <v>4154</v>
+      </c>
+      <c r="L1120" s="36"/>
+      <c r="M1120" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1120" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1120" s="36"/>
+      <c r="P1120" s="36"/>
+      <c r="Q1120" s="36"/>
+    </row>
+    <row r="1121" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1121" s="27"/>
+      <c r="B1121" s="27"/>
+    </row>
+    <row r="1122" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1123" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1124" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1125" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1126" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1127" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1128" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1129" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1130" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1131" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1132" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1133" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1134" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1135" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1136" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1137" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1138" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1139" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1140" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>